<commit_message>
update data base files
</commit_message>
<xml_diff>
--- a/base_datos/inventario/monetized_stock.xlsx
+++ b/base_datos/inventario/monetized_stock.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ407"/>
+  <dimension ref="A1:AR407"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -579,6 +579,9 @@
       <c r="AQ1" s="2" t="n">
         <v>45597</v>
       </c>
+      <c r="AR1" s="2" t="n">
+        <v>45598</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -716,6 +719,7 @@
         <v>7843.47</v>
       </c>
       <c r="AQ2" t="inlineStr"/>
+      <c r="AR2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -850,9 +854,10 @@
         <v>14240.82</v>
       </c>
       <c r="AP3" t="n">
-        <v>14255.06</v>
+        <v>12829.55</v>
       </c>
       <c r="AQ3" t="inlineStr"/>
+      <c r="AR3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -990,6 +995,7 @@
         <v>6414.78</v>
       </c>
       <c r="AQ4" t="inlineStr"/>
+      <c r="AR4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1127,6 +1133,7 @@
         <v>-712.75</v>
       </c>
       <c r="AQ5" t="inlineStr"/>
+      <c r="AR5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1264,6 +1271,7 @@
         <v>1067.71</v>
       </c>
       <c r="AQ6" t="inlineStr"/>
+      <c r="AR6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1401,6 +1409,7 @@
         <v>15532.26</v>
       </c>
       <c r="AQ7" t="inlineStr"/>
+      <c r="AR7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1538,6 +1547,7 @@
         <v>1827.32</v>
       </c>
       <c r="AQ8" t="inlineStr"/>
+      <c r="AR8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1672,9 +1682,10 @@
         <v>14907.9</v>
       </c>
       <c r="AP9" t="n">
-        <v>12933.09</v>
+        <v>14922.8</v>
       </c>
       <c r="AQ9" t="inlineStr"/>
+      <c r="AR9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1812,6 +1823,7 @@
         <v>10943.38</v>
       </c>
       <c r="AQ10" t="inlineStr"/>
+      <c r="AR10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1949,6 +1961,7 @@
         <v>2961451.17</v>
       </c>
       <c r="AQ11" t="inlineStr"/>
+      <c r="AR11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2086,6 +2099,7 @@
         <v>5922902.33</v>
       </c>
       <c r="AQ12" t="inlineStr"/>
+      <c r="AR12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2220,9 +2234,10 @@
         <v>14792470.17</v>
       </c>
       <c r="AP13" t="n">
-        <v>14807255.83</v>
+        <v>10365079.08</v>
       </c>
       <c r="AQ13" t="inlineStr"/>
+      <c r="AR13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -2360,6 +2375,7 @@
         <v>311972.64</v>
       </c>
       <c r="AQ14" t="inlineStr"/>
+      <c r="AR14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2497,6 +2513,7 @@
         <v>12139.02</v>
       </c>
       <c r="AQ15" t="inlineStr"/>
+      <c r="AR15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2634,6 +2651,7 @@
         <v>47818.67</v>
       </c>
       <c r="AQ16" t="inlineStr"/>
+      <c r="AR16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2771,6 +2789,7 @@
         <v>13041.46</v>
       </c>
       <c r="AQ17" t="inlineStr"/>
+      <c r="AR17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2908,6 +2927,7 @@
         <v>0</v>
       </c>
       <c r="AQ18" t="inlineStr"/>
+      <c r="AR18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -3045,6 +3065,7 @@
         <v>23525.94</v>
       </c>
       <c r="AQ19" t="inlineStr"/>
+      <c r="AR19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -3179,9 +3200,10 @@
         <v>25460.99</v>
       </c>
       <c r="AP20" t="n">
-        <v>25486.44</v>
+        <v>21565.45</v>
       </c>
       <c r="AQ20" t="inlineStr"/>
+      <c r="AR20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -3319,6 +3341,7 @@
         <v>9802.48</v>
       </c>
       <c r="AQ21" t="inlineStr"/>
+      <c r="AR21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -3456,6 +3479,7 @@
         <v>52108.08</v>
       </c>
       <c r="AQ22" t="inlineStr"/>
+      <c r="AR22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -3590,9 +3614,10 @@
         <v>55034.44</v>
       </c>
       <c r="AP23" t="n">
-        <v>52190</v>
+        <v>55089.45</v>
       </c>
       <c r="AQ23" t="inlineStr"/>
+      <c r="AR23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -3727,9 +3752,10 @@
         <v>1111.39</v>
       </c>
       <c r="AP24" t="n">
-        <v>635.72</v>
+        <v>1112.51</v>
       </c>
       <c r="AQ24" t="inlineStr"/>
+      <c r="AR24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3864,9 +3890,10 @@
         <v>35163.99</v>
       </c>
       <c r="AP25" t="n">
-        <v>33942.03</v>
+        <v>35199.14</v>
       </c>
       <c r="AQ25" t="inlineStr"/>
+      <c r="AR25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -4001,9 +4028,10 @@
         <v>127335.8</v>
       </c>
       <c r="AP26" t="n">
-        <v>127463.08</v>
+        <v>103563.75</v>
       </c>
       <c r="AQ26" t="inlineStr"/>
+      <c r="AR26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -4141,6 +4169,7 @@
         <v>0</v>
       </c>
       <c r="AQ27" t="inlineStr"/>
+      <c r="AR27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -4278,6 +4307,7 @@
         <v>30278.72</v>
       </c>
       <c r="AQ28" t="inlineStr"/>
+      <c r="AR28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -4412,9 +4442,10 @@
         <v>107914.11</v>
       </c>
       <c r="AP29" t="n">
-        <v>99920.33</v>
+        <v>108021.98</v>
       </c>
       <c r="AQ29" t="inlineStr"/>
+      <c r="AR29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -4549,9 +4580,10 @@
         <v>250231.94</v>
       </c>
       <c r="AP30" t="n">
-        <v>250482.06</v>
+        <v>241536.27</v>
       </c>
       <c r="AQ30" t="inlineStr"/>
+      <c r="AR30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -4686,9 +4718,10 @@
         <v>178527.75</v>
       </c>
       <c r="AP31" t="n">
-        <v>178706.2</v>
+        <v>167051.45</v>
       </c>
       <c r="AQ31" t="inlineStr"/>
+      <c r="AR31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -4823,9 +4856,10 @@
         <v>715481.13</v>
       </c>
       <c r="AP32" t="n">
-        <v>697349.01</v>
+        <v>716196.28</v>
       </c>
       <c r="AQ32" t="inlineStr"/>
+      <c r="AR32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -4960,9 +4994,10 @@
         <v>19389.82</v>
       </c>
       <c r="AP33" t="n">
-        <v>19409.2</v>
+        <v>18196.13</v>
       </c>
       <c r="AQ33" t="inlineStr"/>
+      <c r="AR33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -5100,6 +5135,7 @@
         <v>16419.92</v>
       </c>
       <c r="AQ34" t="inlineStr"/>
+      <c r="AR34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -5237,6 +5273,7 @@
         <v>9679.92</v>
       </c>
       <c r="AQ35" t="inlineStr"/>
+      <c r="AR35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -5374,6 +5411,7 @@
         <v>19559.35</v>
       </c>
       <c r="AQ36" t="inlineStr"/>
+      <c r="AR36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -5511,6 +5549,7 @@
         <v>168291.68</v>
       </c>
       <c r="AQ37" t="inlineStr"/>
+      <c r="AR37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -5648,6 +5687,7 @@
         <v>0</v>
       </c>
       <c r="AQ38" t="inlineStr"/>
+      <c r="AR38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -5785,6 +5825,7 @@
         <v>0</v>
       </c>
       <c r="AQ39" t="inlineStr"/>
+      <c r="AR39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -5922,6 +5963,7 @@
         <v>7643.87</v>
       </c>
       <c r="AQ40" t="inlineStr"/>
+      <c r="AR40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -6056,9 +6098,10 @@
         <v>14375.56</v>
       </c>
       <c r="AP41" t="n">
-        <v>14389.93</v>
+        <v>10278.52</v>
       </c>
       <c r="AQ41" t="inlineStr"/>
+      <c r="AR41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -6196,6 +6239,7 @@
         <v>6041.24</v>
       </c>
       <c r="AQ42" t="inlineStr"/>
+      <c r="AR42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -6333,6 +6377,7 @@
         <v>12273.87</v>
       </c>
       <c r="AQ43" t="inlineStr"/>
+      <c r="AR43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -6470,6 +6515,7 @@
         <v>28700.73</v>
       </c>
       <c r="AQ44" t="inlineStr"/>
+      <c r="AR44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -6607,6 +6653,7 @@
         <v>175303.83</v>
       </c>
       <c r="AQ45" t="inlineStr"/>
+      <c r="AR45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -6741,9 +6788,10 @@
         <v>32369.2</v>
       </c>
       <c r="AP46" t="n">
-        <v>30781.48</v>
+        <v>27541.32</v>
       </c>
       <c r="AQ46" t="inlineStr"/>
+      <c r="AR46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -6881,6 +6929,7 @@
         <v>1247.86</v>
       </c>
       <c r="AQ47" t="inlineStr"/>
+      <c r="AR47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -7018,6 +7067,7 @@
         <v>66273.33</v>
       </c>
       <c r="AQ48" t="inlineStr"/>
+      <c r="AR48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -7155,6 +7205,7 @@
         <v>24596.36</v>
       </c>
       <c r="AQ49" t="inlineStr"/>
+      <c r="AR49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -7289,9 +7340,10 @@
         <v>10576.03</v>
       </c>
       <c r="AP50" t="n">
-        <v>7057.73</v>
+        <v>9410.309999999999</v>
       </c>
       <c r="AQ50" t="inlineStr"/>
+      <c r="AR50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -7429,6 +7481,7 @@
         <v>73016.57000000001</v>
       </c>
       <c r="AQ51" t="inlineStr"/>
+      <c r="AR51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -7566,6 +7619,7 @@
         <v>140909.54</v>
       </c>
       <c r="AQ52" t="inlineStr"/>
+      <c r="AR52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -7700,9 +7754,10 @@
         <v>54423.5</v>
       </c>
       <c r="AP53" t="n">
-        <v>54477.9</v>
+        <v>50846.04</v>
       </c>
       <c r="AQ53" t="inlineStr"/>
+      <c r="AR53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -7840,6 +7895,7 @@
         <v>30870.81</v>
       </c>
       <c r="AQ54" t="inlineStr"/>
+      <c r="AR54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -7977,6 +8033,7 @@
         <v>45398.25</v>
       </c>
       <c r="AQ55" t="inlineStr"/>
+      <c r="AR55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -8114,6 +8171,7 @@
         <v>53109.58</v>
       </c>
       <c r="AQ56" t="inlineStr"/>
+      <c r="AR56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -8251,6 +8309,7 @@
         <v>115072.41</v>
       </c>
       <c r="AQ57" t="inlineStr"/>
+      <c r="AR57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -8385,9 +8444,10 @@
         <v>48500.5</v>
       </c>
       <c r="AP58" t="n">
-        <v>45774.75</v>
+        <v>47161.87</v>
       </c>
       <c r="AQ58" t="inlineStr"/>
+      <c r="AR58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -8525,6 +8585,7 @@
         <v>36064.96</v>
       </c>
       <c r="AQ59" t="inlineStr"/>
+      <c r="AR59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -8659,9 +8720,10 @@
         <v>29640.2</v>
       </c>
       <c r="AP60" t="n">
-        <v>26373.18</v>
+        <v>29669.82</v>
       </c>
       <c r="AQ60" t="inlineStr"/>
+      <c r="AR60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -8796,9 +8858,10 @@
         <v>25137.64</v>
       </c>
       <c r="AP61" t="n">
-        <v>23065.87</v>
+        <v>25162.77</v>
       </c>
       <c r="AQ61" t="inlineStr"/>
+      <c r="AR61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -8933,9 +8996,10 @@
         <v>43440.69</v>
       </c>
       <c r="AP62" t="n">
-        <v>42276.22</v>
+        <v>43484.11</v>
       </c>
       <c r="AQ62" t="inlineStr"/>
+      <c r="AR62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -9070,9 +9134,10 @@
         <v>16098.97</v>
       </c>
       <c r="AP63" t="n">
-        <v>15414.41</v>
+        <v>16115.07</v>
       </c>
       <c r="AQ63" t="inlineStr"/>
+      <c r="AR63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -9210,6 +9275,7 @@
         <v>82569.95</v>
       </c>
       <c r="AQ64" t="inlineStr"/>
+      <c r="AR64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -9347,6 +9413,7 @@
         <v>32824.61</v>
       </c>
       <c r="AQ65" t="inlineStr"/>
+      <c r="AR65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -9481,9 +9548,10 @@
         <v>18435.12</v>
       </c>
       <c r="AP66" t="n">
-        <v>18453.55</v>
+        <v>16146.86</v>
       </c>
       <c r="AQ66" t="inlineStr"/>
+      <c r="AR66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -9621,6 +9689,7 @@
         <v>23077.89</v>
       </c>
       <c r="AQ67" t="inlineStr"/>
+      <c r="AR67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -9755,9 +9824,10 @@
         <v>75452.35000000001</v>
       </c>
       <c r="AP68" t="n">
-        <v>70492.59</v>
+        <v>73010.17999999999</v>
       </c>
       <c r="AQ68" t="inlineStr"/>
+      <c r="AR68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -9895,6 +9965,7 @@
         <v>42713.97</v>
       </c>
       <c r="AQ69" t="inlineStr"/>
+      <c r="AR69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -10029,9 +10100,10 @@
         <v>14453.19</v>
       </c>
       <c r="AP70" t="n">
-        <v>14467.63</v>
+        <v>13089.76</v>
       </c>
       <c r="AQ70" t="inlineStr"/>
+      <c r="AR70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -10166,9 +10238,10 @@
         <v>34077.94</v>
       </c>
       <c r="AP71" t="n">
-        <v>30321.78</v>
+        <v>34112.01</v>
       </c>
       <c r="AQ71" t="inlineStr"/>
+      <c r="AR71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -10306,6 +10379,7 @@
         <v>29133.35</v>
       </c>
       <c r="AQ72" t="inlineStr"/>
+      <c r="AR72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -10443,6 +10517,7 @@
         <v>30761.59</v>
       </c>
       <c r="AQ73" t="inlineStr"/>
+      <c r="AR73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -10577,9 +10652,10 @@
         <v>38768.33</v>
       </c>
       <c r="AP74" t="n">
-        <v>35573.15</v>
+        <v>38807.08</v>
       </c>
       <c r="AQ74" t="inlineStr"/>
+      <c r="AR74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -10717,6 +10793,7 @@
         <v>9085.84</v>
       </c>
       <c r="AQ75" t="inlineStr"/>
+      <c r="AR75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -10854,6 +10931,7 @@
         <v>0</v>
       </c>
       <c r="AQ76" t="inlineStr"/>
+      <c r="AR76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -10991,6 +11069,7 @@
         <v>62215.76</v>
       </c>
       <c r="AQ77" t="inlineStr"/>
+      <c r="AR77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -11125,9 +11204,10 @@
         <v>22750.28</v>
       </c>
       <c r="AP78" t="n">
-        <v>19802.63</v>
+        <v>22773.02</v>
       </c>
       <c r="AQ78" t="inlineStr"/>
+      <c r="AR78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -11265,6 +11345,7 @@
         <v>990.13</v>
       </c>
       <c r="AQ79" t="inlineStr"/>
+      <c r="AR79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -11402,6 +11483,7 @@
         <v>59925.69</v>
       </c>
       <c r="AQ80" t="inlineStr"/>
+      <c r="AR80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -11539,6 +11621,7 @@
         <v>47214.18</v>
       </c>
       <c r="AQ81" t="inlineStr"/>
+      <c r="AR81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -11676,6 +11759,7 @@
         <v>38111.18</v>
       </c>
       <c r="AQ82" t="inlineStr"/>
+      <c r="AR82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -11810,9 +11894,10 @@
         <v>71846.13</v>
       </c>
       <c r="AP83" t="n">
-        <v>71917.95</v>
+        <v>63287.79</v>
       </c>
       <c r="AQ83" t="inlineStr"/>
+      <c r="AR83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -11950,6 +12035,7 @@
         <v>46819.74</v>
       </c>
       <c r="AQ84" t="inlineStr"/>
+      <c r="AR84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -12087,6 +12173,7 @@
         <v>66310.91</v>
       </c>
       <c r="AQ85" t="inlineStr"/>
+      <c r="AR85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -12224,6 +12311,7 @@
         <v>0</v>
       </c>
       <c r="AQ86" t="inlineStr"/>
+      <c r="AR86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -12358,9 +12446,10 @@
         <v>978037.5600000001</v>
       </c>
       <c r="AP87" t="n">
-        <v>851317.52</v>
+        <v>979015.14</v>
       </c>
       <c r="AQ87" t="inlineStr"/>
+      <c r="AR87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -12495,9 +12584,10 @@
         <v>35942.05</v>
       </c>
       <c r="AP88" t="n">
-        <v>28268.41</v>
+        <v>35977.97</v>
       </c>
       <c r="AQ88" t="inlineStr"/>
+      <c r="AR88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -12635,6 +12725,7 @@
         <v>38547.83</v>
       </c>
       <c r="AQ89" t="inlineStr"/>
+      <c r="AR89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -12769,9 +12860,10 @@
         <v>75041.19</v>
       </c>
       <c r="AP90" t="n">
-        <v>75116.19</v>
+        <v>65726.67</v>
       </c>
       <c r="AQ90" t="inlineStr"/>
+      <c r="AR90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -12909,6 +13001,7 @@
         <v>17229.98</v>
       </c>
       <c r="AQ91" t="inlineStr"/>
+      <c r="AR91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -13043,9 +13136,10 @@
         <v>36624.31</v>
       </c>
       <c r="AP92" t="n">
-        <v>36660.92</v>
+        <v>31772.8</v>
       </c>
       <c r="AQ92" t="inlineStr"/>
+      <c r="AR92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -13180,9 +13274,10 @@
         <v>-14493.06</v>
       </c>
       <c r="AP93" t="n">
-        <v>-14507.55</v>
+        <v>-29015.09</v>
       </c>
       <c r="AQ93" t="inlineStr"/>
+      <c r="AR93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -13320,6 +13415,7 @@
         <v>0</v>
       </c>
       <c r="AQ94" t="inlineStr"/>
+      <c r="AR94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -13454,9 +13550,10 @@
         <v>71487.96000000001</v>
       </c>
       <c r="AP95" t="n">
-        <v>66788.78999999999</v>
+        <v>71559.42</v>
       </c>
       <c r="AQ95" t="inlineStr"/>
+      <c r="AR95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -13594,6 +13691,7 @@
         <v>405547.81</v>
       </c>
       <c r="AQ96" t="inlineStr"/>
+      <c r="AR96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -13728,9 +13826,10 @@
         <v>181424.55</v>
       </c>
       <c r="AP97" t="n">
-        <v>181605.89</v>
+        <v>142690.35</v>
       </c>
       <c r="AQ97" t="inlineStr"/>
+      <c r="AR97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -13868,6 +13967,7 @@
         <v>133300.69</v>
       </c>
       <c r="AQ98" t="inlineStr"/>
+      <c r="AR98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -14002,9 +14102,10 @@
         <v>12796.49</v>
       </c>
       <c r="AP99" t="n">
-        <v>8539.52</v>
+        <v>12809.28</v>
       </c>
       <c r="AQ99" t="inlineStr"/>
+      <c r="AR99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -14142,6 +14243,7 @@
         <v>24357.95</v>
       </c>
       <c r="AQ100" t="inlineStr"/>
+      <c r="AR100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -14279,6 +14381,7 @@
         <v>93514.83</v>
       </c>
       <c r="AQ101" t="inlineStr"/>
+      <c r="AR101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -14416,6 +14519,7 @@
         <v>36918.46</v>
       </c>
       <c r="AQ102" t="inlineStr"/>
+      <c r="AR102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -14550,9 +14654,10 @@
         <v>39066.43</v>
       </c>
       <c r="AP103" t="n">
-        <v>39105.48</v>
+        <v>34217.3</v>
       </c>
       <c r="AQ103" t="inlineStr"/>
+      <c r="AR103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -14690,6 +14795,7 @@
         <v>18694.23</v>
       </c>
       <c r="AQ104" t="inlineStr"/>
+      <c r="AR104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -14824,9 +14930,10 @@
         <v>20221.76</v>
       </c>
       <c r="AP105" t="n">
-        <v>20241.97</v>
+        <v>10120.99</v>
       </c>
       <c r="AQ105" t="inlineStr"/>
+      <c r="AR105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -14961,9 +15068,10 @@
         <v>53147.68</v>
       </c>
       <c r="AP106" t="n">
-        <v>43225.65</v>
+        <v>53200.8</v>
       </c>
       <c r="AQ106" t="inlineStr"/>
+      <c r="AR106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -15101,6 +15209,7 @@
         <v>23275.35</v>
       </c>
       <c r="AQ107" t="inlineStr"/>
+      <c r="AR107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -15238,6 +15347,7 @@
         <v>150528.14</v>
       </c>
       <c r="AQ108" t="inlineStr"/>
+      <c r="AR108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -15372,9 +15482,10 @@
         <v>63465.89</v>
       </c>
       <c r="AP109" t="n">
-        <v>63529.33</v>
+        <v>44470.53</v>
       </c>
       <c r="AQ109" t="inlineStr"/>
+      <c r="AR109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -15512,6 +15623,7 @@
         <v>17456.37</v>
       </c>
       <c r="AQ110" t="inlineStr"/>
+      <c r="AR110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -15649,6 +15761,7 @@
         <v>16704.06</v>
       </c>
       <c r="AQ111" t="inlineStr"/>
+      <c r="AR111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -15783,9 +15896,10 @@
         <v>44947.58</v>
       </c>
       <c r="AP112" t="n">
-        <v>42345.89</v>
+        <v>39699.27</v>
       </c>
       <c r="AQ112" t="inlineStr"/>
+      <c r="AR112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -15923,6 +16037,7 @@
         <v>26913.16</v>
       </c>
       <c r="AQ113" t="inlineStr"/>
+      <c r="AR113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -16057,9 +16172,10 @@
         <v>41076.63</v>
       </c>
       <c r="AP114" t="n">
-        <v>41117.69</v>
+        <v>35977.97</v>
       </c>
       <c r="AQ114" t="inlineStr"/>
+      <c r="AR114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -16194,9 +16310,10 @@
         <v>15863.85</v>
       </c>
       <c r="AP115" t="n">
-        <v>11909.78</v>
+        <v>15879.71</v>
       </c>
       <c r="AQ115" t="inlineStr"/>
+      <c r="AR115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -16334,6 +16451,7 @@
         <v>68812.07000000001</v>
       </c>
       <c r="AQ116" t="inlineStr"/>
+      <c r="AR116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -16468,9 +16586,10 @@
         <v>42318.82</v>
       </c>
       <c r="AP117" t="n">
-        <v>35672.52</v>
+        <v>42361.12</v>
       </c>
       <c r="AQ117" t="inlineStr"/>
+      <c r="AR117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -16605,9 +16724,10 @@
         <v>-6681.92</v>
       </c>
       <c r="AP118" t="n">
-        <v>-6688.6</v>
+        <v>-11147.66</v>
       </c>
       <c r="AQ118" t="inlineStr"/>
+      <c r="AR118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -16742,9 +16862,10 @@
         <v>77594.39</v>
       </c>
       <c r="AP119" t="n">
-        <v>64726.62</v>
+        <v>77671.95</v>
       </c>
       <c r="AQ119" t="inlineStr"/>
+      <c r="AR119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -16882,6 +17003,7 @@
         <v>12166.53</v>
       </c>
       <c r="AQ120" t="inlineStr"/>
+      <c r="AR120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -17016,9 +17138,10 @@
         <v>71370.36</v>
       </c>
       <c r="AP121" t="n">
-        <v>60725.44</v>
+        <v>71441.69</v>
       </c>
       <c r="AQ121" t="inlineStr"/>
+      <c r="AR121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -17156,6 +17279,7 @@
         <v>10716.25</v>
       </c>
       <c r="AQ122" t="inlineStr"/>
+      <c r="AR122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -17290,9 +17414,10 @@
         <v>157171.38</v>
       </c>
       <c r="AP123" t="n">
-        <v>157328.48</v>
+        <v>127829.39</v>
       </c>
       <c r="AQ123" t="inlineStr"/>
+      <c r="AR123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -17430,6 +17555,7 @@
         <v>60652.45</v>
       </c>
       <c r="AQ124" t="inlineStr"/>
+      <c r="AR124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -17567,6 +17693,7 @@
         <v>36661.39</v>
       </c>
       <c r="AQ125" t="inlineStr"/>
+      <c r="AR125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -17704,6 +17831,7 @@
         <v>4888.19</v>
       </c>
       <c r="AQ126" t="inlineStr"/>
+      <c r="AR126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -17841,6 +17969,7 @@
         <v>42729.66</v>
       </c>
       <c r="AQ127" t="inlineStr"/>
+      <c r="AR127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -17978,6 +18107,7 @@
         <v>26706.04</v>
       </c>
       <c r="AQ128" t="inlineStr"/>
+      <c r="AR128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -18112,9 +18242,10 @@
         <v>2667.94</v>
       </c>
       <c r="AP129" t="n">
-        <v>-5341.21</v>
+        <v>0</v>
       </c>
       <c r="AQ129" t="inlineStr"/>
+      <c r="AR129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -18252,6 +18383,7 @@
         <v>43225.79</v>
       </c>
       <c r="AQ130" t="inlineStr"/>
+      <c r="AR130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -18389,6 +18521,7 @@
         <v>1051936.97</v>
       </c>
       <c r="AQ131" t="inlineStr"/>
+      <c r="AR131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -18523,9 +18656,10 @@
         <v>262721.64</v>
       </c>
       <c r="AP132" t="n">
-        <v>131492.12</v>
+        <v>262984.24</v>
       </c>
       <c r="AQ132" t="inlineStr"/>
+      <c r="AR132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -18663,6 +18797,7 @@
         <v>95599.85000000001</v>
       </c>
       <c r="AQ133" t="inlineStr"/>
+      <c r="AR133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -18797,9 +18932,10 @@
         <v>0</v>
       </c>
       <c r="AP134" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AQ134" t="inlineStr"/>
+      <c r="AR134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -18937,6 +19073,7 @@
         <v>0</v>
       </c>
       <c r="AQ135" t="inlineStr"/>
+      <c r="AR135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -19071,9 +19208,10 @@
         <v>27848.85</v>
       </c>
       <c r="AP136" t="n">
-        <v>27876.68</v>
+        <v>24159.79</v>
       </c>
       <c r="AQ136" t="inlineStr"/>
+      <c r="AR136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -19211,6 +19349,7 @@
         <v>0</v>
       </c>
       <c r="AQ137" t="inlineStr"/>
+      <c r="AR137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -19348,6 +19487,7 @@
         <v>21542.8</v>
       </c>
       <c r="AQ138" t="inlineStr"/>
+      <c r="AR138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -19485,6 +19625,7 @@
         <v>0</v>
       </c>
       <c r="AQ139" t="inlineStr"/>
+      <c r="AR139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -19622,6 +19763,7 @@
         <v>27442.3</v>
       </c>
       <c r="AQ140" t="inlineStr"/>
+      <c r="AR140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -19759,6 +19901,7 @@
         <v>0</v>
       </c>
       <c r="AQ141" t="inlineStr"/>
+      <c r="AR141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -19896,6 +20039,7 @@
         <v>36195.67</v>
       </c>
       <c r="AQ142" t="inlineStr"/>
+      <c r="AR142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -20033,6 +20177,7 @@
         <v>0</v>
       </c>
       <c r="AQ143" t="inlineStr"/>
+      <c r="AR143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -20167,9 +20312,10 @@
         <v>436030.16</v>
       </c>
       <c r="AP144" t="n">
-        <v>436465.99</v>
+        <v>327349.49</v>
       </c>
       <c r="AQ144" t="inlineStr"/>
+      <c r="AR144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -20307,6 +20453,7 @@
         <v>1702364.75</v>
       </c>
       <c r="AQ145" t="inlineStr"/>
+      <c r="AR145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -20444,6 +20591,7 @@
         <v>0</v>
       </c>
       <c r="AQ146" t="inlineStr"/>
+      <c r="AR146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -20578,9 +20726,10 @@
         <v>335513.06</v>
       </c>
       <c r="AP147" t="n">
-        <v>335848.42</v>
+        <v>321246.31</v>
       </c>
       <c r="AQ147" t="inlineStr"/>
+      <c r="AR147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -20718,6 +20867,7 @@
         <v>262457.99</v>
       </c>
       <c r="AQ148" t="inlineStr"/>
+      <c r="AR148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -20852,9 +21002,10 @@
         <v>45425.94</v>
       </c>
       <c r="AP149" t="n">
-        <v>45471.34</v>
+        <v>40418.97</v>
       </c>
       <c r="AQ149" t="inlineStr"/>
+      <c r="AR149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -20992,6 +21143,7 @@
         <v>0</v>
       </c>
       <c r="AQ150" t="inlineStr"/>
+      <c r="AR150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -21129,6 +21281,7 @@
         <v>18798.52</v>
       </c>
       <c r="AQ151" t="inlineStr"/>
+      <c r="AR151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -21263,9 +21416,10 @@
         <v>11793.66</v>
       </c>
       <c r="AP152" t="n">
-        <v>11805.44</v>
+        <v>7378.4</v>
       </c>
       <c r="AQ152" t="inlineStr"/>
+      <c r="AR152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -21400,9 +21554,10 @@
         <v>26479.69</v>
       </c>
       <c r="AP153" t="n">
-        <v>21204.93</v>
+        <v>26506.16</v>
       </c>
       <c r="AQ153" t="inlineStr"/>
+      <c r="AR153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -21540,6 +21695,7 @@
         <v>105481.96</v>
       </c>
       <c r="AQ154" t="inlineStr"/>
+      <c r="AR154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -21677,6 +21833,7 @@
         <v>139941.64</v>
       </c>
       <c r="AQ155" t="inlineStr"/>
+      <c r="AR155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -21811,9 +21968,10 @@
         <v>2282.87</v>
       </c>
       <c r="AP156" t="n">
-        <v>-1142.58</v>
+        <v>2285.15</v>
       </c>
       <c r="AQ156" t="inlineStr"/>
+      <c r="AR156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -21951,6 +22109,7 @@
         <v>18281.39</v>
       </c>
       <c r="AQ157" t="inlineStr"/>
+      <c r="AR157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -22088,6 +22247,7 @@
         <v>47988.21</v>
       </c>
       <c r="AQ158" t="inlineStr"/>
+      <c r="AR158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -22225,6 +22385,7 @@
         <v>0</v>
       </c>
       <c r="AQ159" t="inlineStr"/>
+      <c r="AR159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -22362,6 +22523,7 @@
         <v>82169.60000000001</v>
       </c>
       <c r="AQ160" t="inlineStr"/>
+      <c r="AR160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -22499,6 +22661,7 @@
         <v>2713.04</v>
       </c>
       <c r="AQ161" t="inlineStr"/>
+      <c r="AR161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -22633,9 +22796,10 @@
         <v>26119.63</v>
       </c>
       <c r="AP162" t="n">
-        <v>26145.74</v>
+        <v>23531.17</v>
       </c>
       <c r="AQ162" t="inlineStr"/>
+      <c r="AR162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -22773,6 +22937,7 @@
         <v>0</v>
       </c>
       <c r="AQ163" t="inlineStr"/>
+      <c r="AR163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -22910,6 +23075,7 @@
         <v>13331.3</v>
       </c>
       <c r="AQ164" t="inlineStr"/>
+      <c r="AR164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -23044,9 +23210,10 @@
         <v>37858.83</v>
       </c>
       <c r="AP165" t="n">
-        <v>32212.17</v>
+        <v>37896.67</v>
       </c>
       <c r="AQ165" t="inlineStr"/>
+      <c r="AR165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -23181,9 +23348,10 @@
         <v>71895.28999999999</v>
       </c>
       <c r="AP166" t="n">
-        <v>71967.16</v>
+        <v>64770.44</v>
       </c>
       <c r="AQ166" t="inlineStr"/>
+      <c r="AR166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -23318,9 +23486,10 @@
         <v>13673.64</v>
       </c>
       <c r="AP167" t="n">
-        <v>11198.71</v>
+        <v>13687.31</v>
       </c>
       <c r="AQ167" t="inlineStr"/>
+      <c r="AR167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -23455,9 +23624,10 @@
         <v>35801.21</v>
       </c>
       <c r="AP168" t="n">
-        <v>31855.11</v>
+        <v>35837</v>
       </c>
       <c r="AQ168" t="inlineStr"/>
+      <c r="AR168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -23595,6 +23765,7 @@
         <v>875725.92</v>
       </c>
       <c r="AQ169" t="inlineStr"/>
+      <c r="AR169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -23732,6 +23903,7 @@
         <v>998632376.89</v>
       </c>
       <c r="AQ170" t="inlineStr"/>
+      <c r="AR170" t="inlineStr"/>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -23869,6 +24041,7 @@
         <v>255284337.01</v>
       </c>
       <c r="AQ171" t="inlineStr"/>
+      <c r="AR171" t="inlineStr"/>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -24006,6 +24179,7 @@
         <v>0</v>
       </c>
       <c r="AQ172" t="inlineStr"/>
+      <c r="AR172" t="inlineStr"/>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -24143,6 +24317,7 @@
         <v>583760.11</v>
       </c>
       <c r="AQ173" t="inlineStr"/>
+      <c r="AR173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -24280,6 +24455,7 @@
         <v>16392.1</v>
       </c>
       <c r="AQ174" t="inlineStr"/>
+      <c r="AR174" t="inlineStr"/>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -24414,9 +24590,10 @@
         <v>0</v>
       </c>
       <c r="AP175" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AQ175" t="inlineStr"/>
+      <c r="AR175" t="inlineStr"/>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -24554,6 +24731,7 @@
         <v>13125.65</v>
       </c>
       <c r="AQ176" t="inlineStr"/>
+      <c r="AR176" t="inlineStr"/>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -24691,6 +24869,7 @@
         <v>18359.01</v>
       </c>
       <c r="AQ177" t="inlineStr"/>
+      <c r="AR177" t="inlineStr"/>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -24828,6 +25007,7 @@
         <v>0</v>
       </c>
       <c r="AQ178" t="inlineStr"/>
+      <c r="AR178" t="inlineStr"/>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -24965,6 +25145,7 @@
         <v>4984.34</v>
       </c>
       <c r="AQ179" t="inlineStr"/>
+      <c r="AR179" t="inlineStr"/>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -25099,9 +25280,10 @@
         <v>85487.7</v>
       </c>
       <c r="AP180" t="n">
-        <v>72737.17999999999</v>
+        <v>85573.14999999999</v>
       </c>
       <c r="AQ180" t="inlineStr"/>
+      <c r="AR180" t="inlineStr"/>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -25236,9 +25418,10 @@
         <v>35540.3</v>
       </c>
       <c r="AP181" t="n">
-        <v>35575.82</v>
+        <v>32839.22</v>
       </c>
       <c r="AQ181" t="inlineStr"/>
+      <c r="AR181" t="inlineStr"/>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -25376,6 +25559,7 @@
         <v>41729.04</v>
       </c>
       <c r="AQ182" t="inlineStr"/>
+      <c r="AR182" t="inlineStr"/>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -25513,6 +25697,7 @@
         <v>14508.05</v>
       </c>
       <c r="AQ183" t="inlineStr"/>
+      <c r="AR183" t="inlineStr"/>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -25647,9 +25832,10 @@
         <v>195852.08</v>
       </c>
       <c r="AP184" t="n">
-        <v>171541.86</v>
+        <v>196047.84</v>
       </c>
       <c r="AQ184" t="inlineStr"/>
+      <c r="AR184" t="inlineStr"/>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -25787,6 +25973,7 @@
         <v>73517.94</v>
       </c>
       <c r="AQ185" t="inlineStr"/>
+      <c r="AR185" t="inlineStr"/>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -25924,6 +26111,7 @@
         <v>30102.62</v>
       </c>
       <c r="AQ186" t="inlineStr"/>
+      <c r="AR186" t="inlineStr"/>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -26061,6 +26249,7 @@
         <v>0</v>
       </c>
       <c r="AQ187" t="inlineStr"/>
+      <c r="AR187" t="inlineStr"/>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -26195,9 +26384,10 @@
         <v>5251290.46</v>
       </c>
       <c r="AP188" t="n">
-        <v>5256539.34</v>
+        <v>5054364.75</v>
       </c>
       <c r="AQ188" t="inlineStr"/>
+      <c r="AR188" t="inlineStr"/>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -26332,9 +26522,10 @@
         <v>2526655.36</v>
       </c>
       <c r="AP189" t="n">
-        <v>2529180.86</v>
+        <v>2371107.05</v>
       </c>
       <c r="AQ189" t="inlineStr"/>
+      <c r="AR189" t="inlineStr"/>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -26472,6 +26663,7 @@
         <v>363904.23</v>
       </c>
       <c r="AQ190" t="inlineStr"/>
+      <c r="AR190" t="inlineStr"/>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -26606,9 +26798,10 @@
         <v>0</v>
       </c>
       <c r="AP191" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AQ191" t="inlineStr"/>
+      <c r="AR191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -26743,9 +26936,10 @@
         <v>87941.74000000001</v>
       </c>
       <c r="AP192" t="n">
-        <v>88029.64</v>
+        <v>76292.36</v>
       </c>
       <c r="AQ192" t="inlineStr"/>
+      <c r="AR192" t="inlineStr"/>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -26880,9 +27074,10 @@
         <v>3316848.64</v>
       </c>
       <c r="AP193" t="n">
-        <v>3162060.92</v>
+        <v>3320163.97</v>
       </c>
       <c r="AQ193" t="inlineStr"/>
+      <c r="AR193" t="inlineStr"/>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -27020,6 +27215,7 @@
         <v>0</v>
       </c>
       <c r="AQ194" t="inlineStr"/>
+      <c r="AR194" t="inlineStr"/>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -27157,6 +27353,7 @@
         <v>0</v>
       </c>
       <c r="AQ195" t="inlineStr"/>
+      <c r="AR195" t="inlineStr"/>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -27294,6 +27491,7 @@
         <v>0</v>
       </c>
       <c r="AQ196" t="inlineStr"/>
+      <c r="AR196" t="inlineStr"/>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -27431,6 +27629,7 @@
         <v>7674.44</v>
       </c>
       <c r="AQ197" t="inlineStr"/>
+      <c r="AR197" t="inlineStr"/>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -27565,9 +27764,10 @@
         <v>61283.88</v>
       </c>
       <c r="AP198" t="n">
-        <v>61345.13</v>
+        <v>56371.2</v>
       </c>
       <c r="AQ198" t="inlineStr"/>
+      <c r="AR198" t="inlineStr"/>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -27702,9 +27902,10 @@
         <v>21532.17</v>
       </c>
       <c r="AP199" t="n">
-        <v>19895.72</v>
+        <v>16579.77</v>
       </c>
       <c r="AQ199" t="inlineStr"/>
+      <c r="AR199" t="inlineStr"/>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -27842,6 +28043,7 @@
         <v>8348.27</v>
       </c>
       <c r="AQ200" t="inlineStr"/>
+      <c r="AR200" t="inlineStr"/>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -27979,6 +28181,7 @@
         <v>0</v>
       </c>
       <c r="AQ201" t="inlineStr"/>
+      <c r="AR201" t="inlineStr"/>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -28116,6 +28319,7 @@
         <v>19079.28</v>
       </c>
       <c r="AQ202" t="inlineStr"/>
+      <c r="AR202" t="inlineStr"/>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -28253,6 +28457,7 @@
         <v>14539.4</v>
       </c>
       <c r="AQ203" t="inlineStr"/>
+      <c r="AR203" t="inlineStr"/>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -28390,6 +28595,7 @@
         <v>12581.64</v>
       </c>
       <c r="AQ204" t="inlineStr"/>
+      <c r="AR204" t="inlineStr"/>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -28527,6 +28733,7 @@
         <v>28965.07</v>
       </c>
       <c r="AQ205" t="inlineStr"/>
+      <c r="AR205" t="inlineStr"/>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -28664,6 +28871,7 @@
         <v>30327.1</v>
       </c>
       <c r="AQ206" t="inlineStr"/>
+      <c r="AR206" t="inlineStr"/>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -28801,6 +29009,7 @@
         <v>6235.48</v>
       </c>
       <c r="AQ207" t="inlineStr"/>
+      <c r="AR207" t="inlineStr"/>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -28935,9 +29144,10 @@
         <v>28557.62</v>
       </c>
       <c r="AP208" t="n">
-        <v>25577.09</v>
+        <v>28586.16</v>
       </c>
       <c r="AQ208" t="inlineStr"/>
+      <c r="AR208" t="inlineStr"/>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -29075,6 +29285,7 @@
         <v>11631.02</v>
       </c>
       <c r="AQ209" t="inlineStr"/>
+      <c r="AR209" t="inlineStr"/>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -29212,6 +29423,7 @@
         <v>24211.76</v>
       </c>
       <c r="AQ210" t="inlineStr"/>
+      <c r="AR210" t="inlineStr"/>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -29349,6 +29561,7 @@
         <v>26211.74</v>
       </c>
       <c r="AQ211" t="inlineStr"/>
+      <c r="AR211" t="inlineStr"/>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -29483,9 +29696,10 @@
         <v>27489.34</v>
       </c>
       <c r="AP212" t="n">
-        <v>27516.81</v>
+        <v>23172.05</v>
       </c>
       <c r="AQ212" t="inlineStr"/>
+      <c r="AR212" t="inlineStr"/>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -29623,6 +29837,7 @@
         <v>8476.32</v>
       </c>
       <c r="AQ213" t="inlineStr"/>
+      <c r="AR213" t="inlineStr"/>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -29757,9 +29972,10 @@
         <v>90338.92999999999</v>
       </c>
       <c r="AP214" t="n">
-        <v>90429.23</v>
+        <v>82893.46000000001</v>
       </c>
       <c r="AQ214" t="inlineStr"/>
+      <c r="AR214" t="inlineStr"/>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -29897,6 +30113,7 @@
         <v>2364.8</v>
       </c>
       <c r="AQ215" t="inlineStr"/>
+      <c r="AR215" t="inlineStr"/>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -30031,9 +30248,10 @@
         <v>11291.61</v>
       </c>
       <c r="AP216" t="n">
-        <v>7535.27</v>
+        <v>11302.9</v>
       </c>
       <c r="AQ216" t="inlineStr"/>
+      <c r="AR216" t="inlineStr"/>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -30171,6 +30389,7 @@
         <v>0</v>
       </c>
       <c r="AQ217" t="inlineStr"/>
+      <c r="AR217" t="inlineStr"/>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -30308,6 +30527,7 @@
         <v>62142.39</v>
       </c>
       <c r="AQ218" t="inlineStr"/>
+      <c r="AR218" t="inlineStr"/>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -30445,6 +30665,7 @@
         <v>78916.39999999999</v>
       </c>
       <c r="AQ219" t="inlineStr"/>
+      <c r="AR219" t="inlineStr"/>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -30579,9 +30800,10 @@
         <v>52880.14</v>
       </c>
       <c r="AP220" t="n">
-        <v>49992.27</v>
+        <v>44110.83</v>
       </c>
       <c r="AQ220" t="inlineStr"/>
+      <c r="AR220" t="inlineStr"/>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -30719,6 +30941,7 @@
         <v>118234.75</v>
       </c>
       <c r="AQ221" t="inlineStr"/>
+      <c r="AR221" t="inlineStr"/>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -30856,6 +31079,7 @@
         <v>0</v>
       </c>
       <c r="AQ222" t="inlineStr"/>
+      <c r="AR222" t="inlineStr"/>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -30993,6 +31217,7 @@
         <v>50921.29</v>
       </c>
       <c r="AQ223" t="inlineStr"/>
+      <c r="AR223" t="inlineStr"/>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -31127,9 +31352,10 @@
         <v>0</v>
       </c>
       <c r="AP224" t="n">
-        <v>-3086.69</v>
+        <v>0</v>
       </c>
       <c r="AQ224" t="inlineStr"/>
+      <c r="AR224" t="inlineStr"/>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -31267,6 +31493,7 @@
         <v>0</v>
       </c>
       <c r="AQ225" t="inlineStr"/>
+      <c r="AR225" t="inlineStr"/>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -31404,6 +31631,7 @@
         <v>0</v>
       </c>
       <c r="AQ226" t="inlineStr"/>
+      <c r="AR226" t="inlineStr"/>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -31538,9 +31766,10 @@
         <v>5249.84</v>
       </c>
       <c r="AP227" t="n">
-        <v>5255.09</v>
+        <v>0</v>
       </c>
       <c r="AQ227" t="inlineStr"/>
+      <c r="AR227" t="inlineStr"/>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -31678,6 +31907,7 @@
         <v>76976.8</v>
       </c>
       <c r="AQ228" t="inlineStr"/>
+      <c r="AR228" t="inlineStr"/>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -31815,6 +32045,7 @@
         <v>103900.87</v>
       </c>
       <c r="AQ229" t="inlineStr"/>
+      <c r="AR229" t="inlineStr"/>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -31952,6 +32183,7 @@
         <v>103715.12</v>
       </c>
       <c r="AQ230" t="inlineStr"/>
+      <c r="AR230" t="inlineStr"/>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -32089,6 +32321,7 @@
         <v>59096.52</v>
       </c>
       <c r="AQ231" t="inlineStr"/>
+      <c r="AR231" t="inlineStr"/>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -32226,6 +32459,7 @@
         <v>10975.41</v>
       </c>
       <c r="AQ232" t="inlineStr"/>
+      <c r="AR232" t="inlineStr"/>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -32363,6 +32597,7 @@
         <v>138581.22</v>
       </c>
       <c r="AQ233" t="inlineStr"/>
+      <c r="AR233" t="inlineStr"/>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -32500,6 +32735,7 @@
         <v>308775.48</v>
       </c>
       <c r="AQ234" t="inlineStr"/>
+      <c r="AR234" t="inlineStr"/>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -32637,6 +32873,7 @@
         <v>207279.98</v>
       </c>
       <c r="AQ235" t="inlineStr"/>
+      <c r="AR235" t="inlineStr"/>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -32774,6 +33011,7 @@
         <v>23499.7</v>
       </c>
       <c r="AQ236" t="inlineStr"/>
+      <c r="AR236" t="inlineStr"/>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -32911,6 +33149,7 @@
         <v>128803.55</v>
       </c>
       <c r="AQ237" t="inlineStr"/>
+      <c r="AR237" t="inlineStr"/>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -33045,9 +33284,10 @@
         <v>16935.72</v>
       </c>
       <c r="AP238" t="n">
-        <v>15069.02</v>
+        <v>16952.65</v>
       </c>
       <c r="AQ238" t="inlineStr"/>
+      <c r="AR238" t="inlineStr"/>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -33185,6 +33425,7 @@
         <v>53704.44</v>
       </c>
       <c r="AQ239" t="inlineStr"/>
+      <c r="AR239" t="inlineStr"/>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -33322,6 +33563,7 @@
         <v>64982.98</v>
       </c>
       <c r="AQ240" t="inlineStr"/>
+      <c r="AR240" t="inlineStr"/>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -33456,9 +33698,10 @@
         <v>6585.89</v>
       </c>
       <c r="AP241" t="n">
-        <v>5650.69</v>
+        <v>6592.48</v>
       </c>
       <c r="AQ241" t="inlineStr"/>
+      <c r="AR241" t="inlineStr"/>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -33596,6 +33839,7 @@
         <v>39541.63</v>
       </c>
       <c r="AQ242" t="inlineStr"/>
+      <c r="AR242" t="inlineStr"/>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -33733,6 +33977,7 @@
         <v>45560.05</v>
       </c>
       <c r="AQ243" t="inlineStr"/>
+      <c r="AR243" t="inlineStr"/>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -33870,6 +34115,7 @@
         <v>27845.52</v>
       </c>
       <c r="AQ244" t="inlineStr"/>
+      <c r="AR244" t="inlineStr"/>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -34007,6 +34253,7 @@
         <v>130675.45</v>
       </c>
       <c r="AQ245" t="inlineStr"/>
+      <c r="AR245" t="inlineStr"/>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -34144,6 +34391,7 @@
         <v>47744.89</v>
       </c>
       <c r="AQ246" t="inlineStr"/>
+      <c r="AR246" t="inlineStr"/>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -34281,6 +34529,7 @@
         <v>110298.63</v>
       </c>
       <c r="AQ247" t="inlineStr"/>
+      <c r="AR247" t="inlineStr"/>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -34418,6 +34667,7 @@
         <v>120729.13</v>
       </c>
       <c r="AQ248" t="inlineStr"/>
+      <c r="AR248" t="inlineStr"/>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -34555,6 +34805,7 @@
         <v>73093.35000000001</v>
       </c>
       <c r="AQ249" t="inlineStr"/>
+      <c r="AR249" t="inlineStr"/>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -34692,6 +34943,7 @@
         <v>233769.66</v>
       </c>
       <c r="AQ250" t="inlineStr"/>
+      <c r="AR250" t="inlineStr"/>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -34829,6 +35081,7 @@
         <v>236764.05</v>
       </c>
       <c r="AQ251" t="inlineStr"/>
+      <c r="AR251" t="inlineStr"/>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -34966,6 +35219,7 @@
         <v>167879.36</v>
       </c>
       <c r="AQ252" t="inlineStr"/>
+      <c r="AR252" t="inlineStr"/>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -35100,9 +35354,10 @@
         <v>712774.85</v>
       </c>
       <c r="AP253" t="n">
-        <v>713487.3</v>
+        <v>682009.92</v>
       </c>
       <c r="AQ253" t="inlineStr"/>
+      <c r="AR253" t="inlineStr"/>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -35240,6 +35495,7 @@
         <v>0</v>
       </c>
       <c r="AQ254" t="inlineStr"/>
+      <c r="AR254" t="inlineStr"/>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -35377,6 +35633,7 @@
         <v>0</v>
       </c>
       <c r="AQ255" t="inlineStr"/>
+      <c r="AR255" t="inlineStr"/>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -35511,9 +35768,10 @@
         <v>40230.44</v>
       </c>
       <c r="AP256" t="n">
-        <v>40270.65</v>
+        <v>36768.85</v>
       </c>
       <c r="AQ256" t="inlineStr"/>
+      <c r="AR256" t="inlineStr"/>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -35648,9 +35906,10 @@
         <v>89637.2</v>
       </c>
       <c r="AP257" t="n">
-        <v>89726.8</v>
+        <v>70499.63</v>
       </c>
       <c r="AQ257" t="inlineStr"/>
+      <c r="AR257" t="inlineStr"/>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -35785,9 +36044,10 @@
         <v>13251.52</v>
       </c>
       <c r="AP258" t="n">
-        <v>13264.77</v>
+        <v>12058.88</v>
       </c>
       <c r="AQ258" t="inlineStr"/>
+      <c r="AR258" t="inlineStr"/>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -35925,6 +36185,7 @@
         <v>0</v>
       </c>
       <c r="AQ259" t="inlineStr"/>
+      <c r="AR259" t="inlineStr"/>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -36062,6 +36323,7 @@
         <v>6883.22</v>
       </c>
       <c r="AQ260" t="inlineStr"/>
+      <c r="AR260" t="inlineStr"/>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -36196,9 +36458,10 @@
         <v>6122.32</v>
       </c>
       <c r="AP261" t="n">
-        <v>3501.96</v>
+        <v>6128.44</v>
       </c>
       <c r="AQ261" t="inlineStr"/>
+      <c r="AR261" t="inlineStr"/>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -36333,9 +36596,10 @@
         <v>34987.18</v>
       </c>
       <c r="AP262" t="n">
-        <v>33271.05</v>
+        <v>35022.15</v>
       </c>
       <c r="AQ262" t="inlineStr"/>
+      <c r="AR262" t="inlineStr"/>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -36473,6 +36737,7 @@
         <v>52650.33</v>
       </c>
       <c r="AQ263" t="inlineStr"/>
+      <c r="AR263" t="inlineStr"/>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -36607,9 +36872,10 @@
         <v>47482.54</v>
       </c>
       <c r="AP264" t="n">
-        <v>41588.75</v>
+        <v>47530.01</v>
       </c>
       <c r="AQ264" t="inlineStr"/>
+      <c r="AR264" t="inlineStr"/>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
@@ -36747,6 +37013,7 @@
         <v>43956.4</v>
       </c>
       <c r="AQ265" t="inlineStr"/>
+      <c r="AR265" t="inlineStr"/>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
@@ -36881,9 +37148,10 @@
         <v>27987.73</v>
       </c>
       <c r="AP266" t="n">
-        <v>28015.71</v>
+        <v>22762.76</v>
       </c>
       <c r="AQ266" t="inlineStr"/>
+      <c r="AR266" t="inlineStr"/>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
@@ -37021,6 +37289,7 @@
         <v>32115.24</v>
       </c>
       <c r="AQ267" t="inlineStr"/>
+      <c r="AR267" t="inlineStr"/>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -37155,9 +37424,10 @@
         <v>5642.75</v>
       </c>
       <c r="AP268" t="n">
-        <v>5648.39</v>
+        <v>4942.34</v>
       </c>
       <c r="AQ268" t="inlineStr"/>
+      <c r="AR268" t="inlineStr"/>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -37292,9 +37562,10 @@
         <v>1410.69</v>
       </c>
       <c r="AP269" t="n">
-        <v>0</v>
+        <v>1412.1</v>
       </c>
       <c r="AQ269" t="inlineStr"/>
+      <c r="AR269" t="inlineStr"/>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -37429,9 +37700,10 @@
         <v>5642.75</v>
       </c>
       <c r="AP270" t="n">
-        <v>5648.39</v>
+        <v>3530.24</v>
       </c>
       <c r="AQ270" t="inlineStr"/>
+      <c r="AR270" t="inlineStr"/>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
@@ -37569,6 +37841,7 @@
         <v>6603.01</v>
       </c>
       <c r="AQ271" t="inlineStr"/>
+      <c r="AR271" t="inlineStr"/>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
@@ -37706,6 +37979,7 @@
         <v>-660.3</v>
       </c>
       <c r="AQ272" t="inlineStr"/>
+      <c r="AR272" t="inlineStr"/>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
@@ -37843,6 +38117,7 @@
         <v>10670.52</v>
       </c>
       <c r="AQ273" t="inlineStr"/>
+      <c r="AR273" t="inlineStr"/>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
@@ -37980,6 +38255,7 @@
         <v>13414.91</v>
       </c>
       <c r="AQ274" t="inlineStr"/>
+      <c r="AR274" t="inlineStr"/>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -38114,9 +38390,10 @@
         <v>5642.75</v>
       </c>
       <c r="AP275" t="n">
-        <v>4236.29</v>
+        <v>5648.39</v>
       </c>
       <c r="AQ275" t="inlineStr"/>
+      <c r="AR275" t="inlineStr"/>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -38254,6 +38531,7 @@
         <v>16922.24</v>
       </c>
       <c r="AQ276" t="inlineStr"/>
+      <c r="AR276" t="inlineStr"/>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -38391,6 +38669,7 @@
         <v>0</v>
       </c>
       <c r="AQ277" t="inlineStr"/>
+      <c r="AR277" t="inlineStr"/>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
@@ -38528,6 +38807,7 @@
         <v>39556.18</v>
       </c>
       <c r="AQ278" t="inlineStr"/>
+      <c r="AR278" t="inlineStr"/>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -38665,6 +38945,7 @@
         <v>20383.16</v>
       </c>
       <c r="AQ279" t="inlineStr"/>
+      <c r="AR279" t="inlineStr"/>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -38802,6 +39083,7 @@
         <v>6412.41</v>
       </c>
       <c r="AQ280" t="inlineStr"/>
+      <c r="AR280" t="inlineStr"/>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -38936,9 +39218,10 @@
         <v>2669.13</v>
       </c>
       <c r="AP281" t="n">
-        <v>2671.8</v>
+        <v>2337.83</v>
       </c>
       <c r="AQ281" t="inlineStr"/>
+      <c r="AR281" t="inlineStr"/>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -39073,9 +39356,10 @@
         <v>29277.75</v>
       </c>
       <c r="AP282" t="n">
-        <v>29307.02</v>
+        <v>27353.21</v>
       </c>
       <c r="AQ282" t="inlineStr"/>
+      <c r="AR282" t="inlineStr"/>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
@@ -39213,6 +39497,7 @@
         <v>4884.5</v>
       </c>
       <c r="AQ283" t="inlineStr"/>
+      <c r="AR283" t="inlineStr"/>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
@@ -39350,6 +39635,7 @@
         <v>8792.1</v>
       </c>
       <c r="AQ284" t="inlineStr"/>
+      <c r="AR284" t="inlineStr"/>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
@@ -39487,6 +39773,7 @@
         <v>1953.8</v>
       </c>
       <c r="AQ285" t="inlineStr"/>
+      <c r="AR285" t="inlineStr"/>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
@@ -39624,6 +39911,7 @@
         <v>3907.6</v>
       </c>
       <c r="AQ286" t="inlineStr"/>
+      <c r="AR286" t="inlineStr"/>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
@@ -39761,6 +40049,7 @@
         <v>95796.50999999999</v>
       </c>
       <c r="AQ287" t="inlineStr"/>
+      <c r="AR287" t="inlineStr"/>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
@@ -39898,6 +40187,7 @@
         <v>8059114.53</v>
       </c>
       <c r="AQ288" t="inlineStr"/>
+      <c r="AR288" t="inlineStr"/>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
@@ -40035,6 +40325,7 @@
         <v>0</v>
       </c>
       <c r="AQ289" t="inlineStr"/>
+      <c r="AR289" t="inlineStr"/>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
@@ -40172,6 +40463,7 @@
         <v>876860613.48</v>
       </c>
       <c r="AQ290" t="inlineStr"/>
+      <c r="AR290" t="inlineStr"/>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
@@ -40306,9 +40598,10 @@
         <v>47383.6</v>
       </c>
       <c r="AP291" t="n">
-        <v>47430.96</v>
+        <v>41502.09</v>
       </c>
       <c r="AQ291" t="inlineStr"/>
+      <c r="AR291" t="inlineStr"/>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
@@ -40446,6 +40739,7 @@
         <v>242025.8</v>
       </c>
       <c r="AQ292" t="inlineStr"/>
+      <c r="AR292" t="inlineStr"/>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
@@ -40580,9 +40874,10 @@
         <v>141040.74</v>
       </c>
       <c r="AP293" t="n">
-        <v>80675.27</v>
+        <v>141181.72</v>
       </c>
       <c r="AQ293" t="inlineStr"/>
+      <c r="AR293" t="inlineStr"/>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
@@ -40717,9 +41012,10 @@
         <v>40297.36</v>
       </c>
       <c r="AP294" t="n">
-        <v>40337.63</v>
+        <v>-20168.82</v>
       </c>
       <c r="AQ294" t="inlineStr"/>
+      <c r="AR294" t="inlineStr"/>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
@@ -40857,6 +41153,7 @@
         <v>-20168.82</v>
       </c>
       <c r="AQ295" t="inlineStr"/>
+      <c r="AR295" t="inlineStr"/>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
@@ -40991,9 +41288,10 @@
         <v>8145.95</v>
       </c>
       <c r="AP296" t="n">
-        <v>6715.13</v>
+        <v>8154.09</v>
       </c>
       <c r="AQ296" t="inlineStr"/>
+      <c r="AR296" t="inlineStr"/>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
@@ -41128,9 +41426,10 @@
         <v>94581.87</v>
       </c>
       <c r="AP297" t="n">
-        <v>92367.23</v>
+        <v>94676.41</v>
       </c>
       <c r="AQ297" t="inlineStr"/>
+      <c r="AR297" t="inlineStr"/>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
@@ -41268,6 +41567,7 @@
         <v>0</v>
       </c>
       <c r="AQ298" t="inlineStr"/>
+      <c r="AR298" t="inlineStr"/>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
@@ -41405,6 +41705,7 @@
         <v>18650.35</v>
       </c>
       <c r="AQ299" t="inlineStr"/>
+      <c r="AR299" t="inlineStr"/>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
@@ -41542,6 +41843,7 @@
         <v>9944.84</v>
       </c>
       <c r="AQ300" t="inlineStr"/>
+      <c r="AR300" t="inlineStr"/>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
@@ -41679,6 +41981,7 @@
         <v>44969.37</v>
       </c>
       <c r="AQ301" t="inlineStr"/>
+      <c r="AR301" t="inlineStr"/>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
@@ -41816,6 +42119,7 @@
         <v>225921.35</v>
       </c>
       <c r="AQ302" t="inlineStr"/>
+      <c r="AR302" t="inlineStr"/>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
@@ -41953,6 +42257,7 @@
         <v>4286.59</v>
       </c>
       <c r="AQ303" t="inlineStr"/>
+      <c r="AR303" t="inlineStr"/>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
@@ -42087,9 +42392,10 @@
         <v>4803.7</v>
       </c>
       <c r="AP304" t="n">
-        <v>3497.1</v>
+        <v>4808.51</v>
       </c>
       <c r="AQ304" t="inlineStr"/>
+      <c r="AR304" t="inlineStr"/>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
@@ -42224,9 +42530,10 @@
         <v>24006.36</v>
       </c>
       <c r="AP305" t="n">
-        <v>23069.14</v>
+        <v>24030.36</v>
       </c>
       <c r="AQ305" t="inlineStr"/>
+      <c r="AR305" t="inlineStr"/>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
@@ -42361,9 +42668,10 @@
         <v>0</v>
       </c>
       <c r="AP306" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AQ306" t="inlineStr"/>
+      <c r="AR306" t="inlineStr"/>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
@@ -42501,6 +42809,7 @@
         <v>47846799.07</v>
       </c>
       <c r="AQ307" t="inlineStr"/>
+      <c r="AR307" t="inlineStr"/>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
@@ -42635,9 +42944,10 @@
         <v>389697.85</v>
       </c>
       <c r="AP308" t="n">
-        <v>390087.36</v>
+        <v>348500.23</v>
       </c>
       <c r="AQ308" t="inlineStr"/>
+      <c r="AR308" t="inlineStr"/>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
@@ -42775,6 +43085,7 @@
         <v>252162.15</v>
       </c>
       <c r="AQ309" t="inlineStr"/>
+      <c r="AR309" t="inlineStr"/>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
@@ -42912,6 +43223,7 @@
         <v>31284971.57</v>
       </c>
       <c r="AQ310" t="inlineStr"/>
+      <c r="AR310" t="inlineStr"/>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
@@ -43049,6 +43361,7 @@
         <v>10472678.9</v>
       </c>
       <c r="AQ311" t="inlineStr"/>
+      <c r="AR311" t="inlineStr"/>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
@@ -43183,9 +43496,10 @@
         <v>11441325.87</v>
       </c>
       <c r="AP312" t="n">
-        <v>11452761.93</v>
+        <v>10889511.34</v>
       </c>
       <c r="AQ312" t="inlineStr"/>
+      <c r="AR312" t="inlineStr"/>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
@@ -43323,6 +43637,7 @@
         <v>86094.78999999999</v>
       </c>
       <c r="AQ313" t="inlineStr"/>
+      <c r="AR313" t="inlineStr"/>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
@@ -43460,6 +43775,7 @@
         <v>315364.64</v>
       </c>
       <c r="AQ314" t="inlineStr"/>
+      <c r="AR314" t="inlineStr"/>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
@@ -43594,9 +43910,10 @@
         <v>14560.31</v>
       </c>
       <c r="AP315" t="n">
-        <v>-14574.87</v>
+        <v>14574.87</v>
       </c>
       <c r="AQ315" t="inlineStr"/>
+      <c r="AR315" t="inlineStr"/>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
@@ -43734,6 +44051,7 @@
         <v>0</v>
       </c>
       <c r="AQ316" t="inlineStr"/>
+      <c r="AR316" t="inlineStr"/>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
@@ -43868,9 +44186,10 @@
         <v>19867.74</v>
       </c>
       <c r="AP317" t="n">
-        <v>13258.4</v>
+        <v>19887.6</v>
       </c>
       <c r="AQ317" t="inlineStr"/>
+      <c r="AR317" t="inlineStr"/>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
@@ -44005,9 +44324,10 @@
         <v>16190827.51</v>
       </c>
       <c r="AP318" t="n">
-        <v>16207010.89</v>
+        <v>15801835.62</v>
       </c>
       <c r="AQ318" t="inlineStr"/>
+      <c r="AR318" t="inlineStr"/>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
@@ -44145,6 +44465,7 @@
         <v>1684778.21</v>
       </c>
       <c r="AQ319" t="inlineStr"/>
+      <c r="AR319" t="inlineStr"/>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
@@ -44282,6 +44603,7 @@
         <v>445777.63</v>
       </c>
       <c r="AQ320" t="inlineStr"/>
+      <c r="AR320" t="inlineStr"/>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
@@ -44416,9 +44738,10 @@
         <v>78120.23</v>
       </c>
       <c r="AP321" t="n">
-        <v>78198.31</v>
+        <v>52132.21</v>
       </c>
       <c r="AQ321" t="inlineStr"/>
+      <c r="AR321" t="inlineStr"/>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
@@ -44556,6 +44879,7 @@
         <v>114491.04</v>
       </c>
       <c r="AQ322" t="inlineStr"/>
+      <c r="AR322" t="inlineStr"/>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
@@ -44693,6 +45017,7 @@
         <v>6033994.82</v>
       </c>
       <c r="AQ323" t="inlineStr"/>
+      <c r="AR323" t="inlineStr"/>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
@@ -44830,6 +45155,7 @@
         <v>463392.5</v>
       </c>
       <c r="AQ324" t="inlineStr"/>
+      <c r="AR324" t="inlineStr"/>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
@@ -44967,6 +45293,7 @@
         <v>0</v>
       </c>
       <c r="AQ325" t="inlineStr"/>
+      <c r="AR325" t="inlineStr"/>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
@@ -45104,6 +45431,7 @@
         <v>28478.85</v>
       </c>
       <c r="AQ326" t="inlineStr"/>
+      <c r="AR326" t="inlineStr"/>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
@@ -45241,6 +45569,7 @@
         <v>343624.4</v>
       </c>
       <c r="AQ327" t="inlineStr"/>
+      <c r="AR327" t="inlineStr"/>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
@@ -45378,6 +45707,7 @@
         <v>9897853.08</v>
       </c>
       <c r="AQ328" t="inlineStr"/>
+      <c r="AR328" t="inlineStr"/>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
@@ -45515,6 +45845,7 @@
         <v>0</v>
       </c>
       <c r="AQ329" t="inlineStr"/>
+      <c r="AR329" t="inlineStr"/>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
@@ -45649,9 +45980,10 @@
         <v>95723.03999999999</v>
       </c>
       <c r="AP330" t="n">
-        <v>76654.98</v>
+        <v>95818.72</v>
       </c>
       <c r="AQ330" t="inlineStr"/>
+      <c r="AR330" t="inlineStr"/>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
@@ -45789,6 +46121,7 @@
         <v>1478248.49</v>
       </c>
       <c r="AQ331" t="inlineStr"/>
+      <c r="AR331" t="inlineStr"/>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
@@ -45926,6 +46259,7 @@
         <v>0</v>
       </c>
       <c r="AQ332" t="inlineStr"/>
+      <c r="AR332" t="inlineStr"/>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
@@ -46063,6 +46397,7 @@
         <v>0</v>
       </c>
       <c r="AQ333" t="inlineStr"/>
+      <c r="AR333" t="inlineStr"/>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
@@ -46200,6 +46535,7 @@
         <v>0</v>
       </c>
       <c r="AQ334" t="inlineStr"/>
+      <c r="AR334" t="inlineStr"/>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
@@ -46334,9 +46670,10 @@
         <v>3500547.86</v>
       </c>
       <c r="AP335" t="n">
-        <v>3504046.8</v>
+        <v>3378902.27</v>
       </c>
       <c r="AQ335" t="inlineStr"/>
+      <c r="AR335" t="inlineStr"/>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
@@ -46474,6 +46811,7 @@
         <v>208574.21</v>
       </c>
       <c r="AQ336" t="inlineStr"/>
+      <c r="AR336" t="inlineStr"/>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
@@ -46611,6 +46949,7 @@
         <v>125144.53</v>
       </c>
       <c r="AQ337" t="inlineStr"/>
+      <c r="AR337" t="inlineStr"/>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
@@ -46748,6 +47087,7 @@
         <v>-166859.37</v>
       </c>
       <c r="AQ338" t="inlineStr"/>
+      <c r="AR338" t="inlineStr"/>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
@@ -46882,9 +47222,10 @@
         <v>1562126.28</v>
       </c>
       <c r="AP339" t="n">
-        <v>1563687.68</v>
+        <v>1429657.31</v>
       </c>
       <c r="AQ339" t="inlineStr"/>
+      <c r="AR339" t="inlineStr"/>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
@@ -47022,6 +47363,7 @@
         <v>-89353.58</v>
       </c>
       <c r="AQ340" t="inlineStr"/>
+      <c r="AR340" t="inlineStr"/>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
@@ -47159,6 +47501,7 @@
         <v>1927234.12</v>
       </c>
       <c r="AQ341" t="inlineStr"/>
+      <c r="AR341" t="inlineStr"/>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
@@ -47296,6 +47639,7 @@
         <v>90719.66</v>
       </c>
       <c r="AQ342" t="inlineStr"/>
+      <c r="AR342" t="inlineStr"/>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
@@ -47433,6 +47777,7 @@
         <v>5313.61</v>
       </c>
       <c r="AQ343" t="inlineStr"/>
+      <c r="AR343" t="inlineStr"/>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
@@ -47570,6 +47915,7 @@
         <v>69816.2</v>
       </c>
       <c r="AQ344" t="inlineStr"/>
+      <c r="AR344" t="inlineStr"/>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
@@ -47704,9 +48050,10 @@
         <v>-4900.79</v>
       </c>
       <c r="AP345" t="n">
-        <v>-4905.69</v>
+        <v>-12264.22</v>
       </c>
       <c r="AQ345" t="inlineStr"/>
+      <c r="AR345" t="inlineStr"/>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
@@ -47844,6 +48191,7 @@
         <v>91856.41</v>
       </c>
       <c r="AQ346" t="inlineStr"/>
+      <c r="AR346" t="inlineStr"/>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
@@ -47981,6 +48329,7 @@
         <v>3924.58</v>
       </c>
       <c r="AQ347" t="inlineStr"/>
+      <c r="AR347" t="inlineStr"/>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
@@ -48115,9 +48464,10 @@
         <v>839228.55</v>
       </c>
       <c r="AP348" t="n">
-        <v>840067.4</v>
+        <v>795853.3199999999</v>
       </c>
       <c r="AQ348" t="inlineStr"/>
+      <c r="AR348" t="inlineStr"/>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
@@ -48248,9 +48598,10 @@
         <v>6990015.68</v>
       </c>
       <c r="AP349" t="n">
-        <v>6997002.48</v>
+        <v>6608280.12</v>
       </c>
       <c r="AQ349" t="inlineStr"/>
+      <c r="AR349" t="inlineStr"/>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
@@ -48388,6 +48739,7 @@
         <v>6906283.41</v>
       </c>
       <c r="AQ350" t="inlineStr"/>
+      <c r="AR350" t="inlineStr"/>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
@@ -48525,6 +48877,7 @@
         <v>20126546.09</v>
       </c>
       <c r="AQ351" t="inlineStr"/>
+      <c r="AR351" t="inlineStr"/>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
@@ -48659,9 +49012,10 @@
         <v>45877806.8</v>
       </c>
       <c r="AP352" t="n">
-        <v>45884974.66</v>
+        <v>45923663.51</v>
       </c>
       <c r="AQ352" t="inlineStr"/>
+      <c r="AR352" t="inlineStr"/>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
@@ -48796,9 +49150,10 @@
         <v>8086.01</v>
       </c>
       <c r="AP353" t="n">
-        <v>6070.57</v>
+        <v>8094.09</v>
       </c>
       <c r="AQ353" t="inlineStr"/>
+      <c r="AR353" t="inlineStr"/>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
@@ -48936,6 +49291,7 @@
         <v>5614126.56</v>
       </c>
       <c r="AQ354" t="inlineStr"/>
+      <c r="AR354" t="inlineStr"/>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
@@ -49070,9 +49426,10 @@
         <v>16290209.28</v>
       </c>
       <c r="AP355" t="n">
-        <v>16257078.39</v>
+        <v>16281785.2</v>
       </c>
       <c r="AQ355" t="inlineStr"/>
+      <c r="AR355" t="inlineStr"/>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
@@ -49210,6 +49567,7 @@
         <v>24332507.49</v>
       </c>
       <c r="AQ356" t="inlineStr"/>
+      <c r="AR356" t="inlineStr"/>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
@@ -49344,9 +49702,10 @@
         <v>218773894.07</v>
       </c>
       <c r="AP357" t="n">
-        <v>194660059.88</v>
+        <v>218992567.37</v>
       </c>
       <c r="AQ357" t="inlineStr"/>
+      <c r="AR357" t="inlineStr"/>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
@@ -49481,9 +49840,10 @@
         <v>1129055.43</v>
       </c>
       <c r="AP358" t="n">
-        <v>1130183.97</v>
+        <v>1127137.65</v>
       </c>
       <c r="AQ358" t="inlineStr"/>
+      <c r="AR358" t="inlineStr"/>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
@@ -49618,9 +49978,10 @@
         <v>4020046.64</v>
       </c>
       <c r="AP359" t="n">
-        <v>3977811.22</v>
+        <v>4024064.84</v>
       </c>
       <c r="AQ359" t="inlineStr"/>
+      <c r="AR359" t="inlineStr"/>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
@@ -49755,9 +50116,10 @@
         <v>126036.37</v>
       </c>
       <c r="AP360" t="n">
-        <v>126162.35</v>
+        <v>118277.2</v>
       </c>
       <c r="AQ360" t="inlineStr"/>
+      <c r="AR360" t="inlineStr"/>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
@@ -49892,9 +50254,10 @@
         <v>130300.85</v>
       </c>
       <c r="AP361" t="n">
-        <v>130431.09</v>
+        <v>118573.72</v>
       </c>
       <c r="AQ361" t="inlineStr"/>
+      <c r="AR361" t="inlineStr"/>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
@@ -50032,6 +50395,7 @@
         <v>13860.54</v>
       </c>
       <c r="AQ362" t="inlineStr"/>
+      <c r="AR362" t="inlineStr"/>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
@@ -50169,6 +50533,7 @@
         <v>51383.68</v>
       </c>
       <c r="AQ363" t="inlineStr"/>
+      <c r="AR363" t="inlineStr"/>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
@@ -50306,6 +50671,7 @@
         <v>216342.02</v>
       </c>
       <c r="AQ364" t="inlineStr"/>
+      <c r="AR364" t="inlineStr"/>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
@@ -50440,9 +50806,10 @@
         <v>292331.61</v>
       </c>
       <c r="AP365" t="n">
-        <v>292623.81</v>
+        <v>284643.16</v>
       </c>
       <c r="AQ365" t="inlineStr"/>
+      <c r="AR365" t="inlineStr"/>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
@@ -50577,9 +50944,10 @@
         <v>1293808.11</v>
       </c>
       <c r="AP366" t="n">
-        <v>1295101.33</v>
+        <v>1248847.71</v>
       </c>
       <c r="AQ366" t="inlineStr"/>
+      <c r="AR366" t="inlineStr"/>
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
@@ -50717,6 +51085,7 @@
         <v>42048.74</v>
       </c>
       <c r="AQ367" t="inlineStr"/>
+      <c r="AR367" t="inlineStr"/>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
@@ -50851,9 +51220,10 @@
         <v>1562789.72</v>
       </c>
       <c r="AP368" t="n">
-        <v>1545728.56</v>
+        <v>1527105.32</v>
       </c>
       <c r="AQ368" t="inlineStr"/>
+      <c r="AR368" t="inlineStr"/>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
@@ -50988,9 +51358,10 @@
         <v>20419.95</v>
       </c>
       <c r="AP369" t="n">
-        <v>14308.25</v>
+        <v>20440.36</v>
       </c>
       <c r="AQ369" t="inlineStr"/>
+      <c r="AR369" t="inlineStr"/>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
@@ -51125,9 +51496,10 @@
         <v>872553.4</v>
       </c>
       <c r="AP370" t="n">
-        <v>873425.55</v>
+        <v>841076.46</v>
       </c>
       <c r="AQ370" t="inlineStr"/>
+      <c r="AR370" t="inlineStr"/>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
@@ -51265,6 +51637,7 @@
         <v>3237759.2</v>
       </c>
       <c r="AQ371" t="inlineStr"/>
+      <c r="AR371" t="inlineStr"/>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
@@ -51402,6 +51775,7 @@
         <v>617019.62</v>
       </c>
       <c r="AQ372" t="inlineStr"/>
+      <c r="AR372" t="inlineStr"/>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
@@ -51536,9 +51910,10 @@
         <v>24656.14</v>
       </c>
       <c r="AP373" t="n">
-        <v>0</v>
+        <v>24680.78</v>
       </c>
       <c r="AQ373" t="inlineStr"/>
+      <c r="AR373" t="inlineStr"/>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
@@ -51676,6 +52051,7 @@
         <v>144608.18</v>
       </c>
       <c r="AQ374" t="inlineStr"/>
+      <c r="AR374" t="inlineStr"/>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
@@ -51813,6 +52189,7 @@
         <v>455655.48</v>
       </c>
       <c r="AQ375" t="inlineStr"/>
+      <c r="AR375" t="inlineStr"/>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
@@ -51950,6 +52327,7 @@
         <v>23276.26</v>
       </c>
       <c r="AQ376" t="inlineStr"/>
+      <c r="AR376" t="inlineStr"/>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
@@ -52087,6 +52465,7 @@
         <v>285169.71</v>
       </c>
       <c r="AQ377" t="inlineStr"/>
+      <c r="AR377" t="inlineStr"/>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
@@ -52221,9 +52600,10 @@
         <v>136324.79</v>
       </c>
       <c r="AP378" t="n">
-        <v>136461.06</v>
+        <v>133428.59</v>
       </c>
       <c r="AQ378" t="inlineStr"/>
+      <c r="AR378" t="inlineStr"/>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
@@ -52361,6 +52741,7 @@
         <v>2406414.6</v>
       </c>
       <c r="AQ379" t="inlineStr"/>
+      <c r="AR379" t="inlineStr"/>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
@@ -52498,6 +52879,7 @@
         <v>115975.73</v>
       </c>
       <c r="AQ380" t="inlineStr"/>
+      <c r="AR380" t="inlineStr"/>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
@@ -52635,6 +53017,7 @@
         <v>634410.4300000001</v>
       </c>
       <c r="AQ381" t="inlineStr"/>
+      <c r="AR381" t="inlineStr"/>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
@@ -52772,6 +53155,7 @@
         <v>868305.6899999999</v>
       </c>
       <c r="AQ382" t="inlineStr"/>
+      <c r="AR382" t="inlineStr"/>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
@@ -52909,6 +53293,7 @@
         <v>608235</v>
       </c>
       <c r="AQ383" t="inlineStr"/>
+      <c r="AR383" t="inlineStr"/>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
@@ -53043,9 +53428,10 @@
         <v>404116.17</v>
       </c>
       <c r="AP384" t="n">
-        <v>371721.17</v>
+        <v>404520.1</v>
       </c>
       <c r="AQ384" t="inlineStr"/>
+      <c r="AR384" t="inlineStr"/>
     </row>
     <row r="385">
       <c r="A385" t="inlineStr">
@@ -53183,6 +53569,7 @@
         <v>251198.42</v>
       </c>
       <c r="AQ385" t="inlineStr"/>
+      <c r="AR385" t="inlineStr"/>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
@@ -53317,9 +53704,10 @@
         <v>927139.64</v>
       </c>
       <c r="AP386" t="n">
-        <v>906483.41</v>
+        <v>928066.35</v>
       </c>
       <c r="AQ386" t="inlineStr"/>
+      <c r="AR386" t="inlineStr"/>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">
@@ -53457,6 +53845,7 @@
         <v>331502.57</v>
       </c>
       <c r="AQ387" t="inlineStr"/>
+      <c r="AR387" t="inlineStr"/>
     </row>
     <row r="388">
       <c r="A388" t="inlineStr">
@@ -53594,6 +53983,7 @@
         <v>89900.53</v>
       </c>
       <c r="AQ388" t="inlineStr"/>
+      <c r="AR388" t="inlineStr"/>
     </row>
     <row r="389">
       <c r="A389" t="inlineStr">
@@ -53731,6 +54121,7 @@
         <v>7541960.3</v>
       </c>
       <c r="AQ389" t="inlineStr"/>
+      <c r="AR389" t="inlineStr"/>
     </row>
     <row r="390">
       <c r="A390" t="inlineStr">
@@ -53865,9 +54256,10 @@
         <v>6302818.04</v>
       </c>
       <c r="AP390" t="n">
-        <v>6309117.96</v>
+        <v>6091562.17</v>
       </c>
       <c r="AQ390" t="inlineStr"/>
+      <c r="AR390" t="inlineStr"/>
     </row>
     <row r="391">
       <c r="A391" t="inlineStr">
@@ -54005,6 +54397,7 @@
         <v>36434.86</v>
       </c>
       <c r="AQ391" t="inlineStr"/>
+      <c r="AR391" t="inlineStr"/>
     </row>
     <row r="392">
       <c r="A392" t="inlineStr">
@@ -54142,6 +54535,7 @@
         <v>246935.88</v>
       </c>
       <c r="AQ392" t="inlineStr"/>
+      <c r="AR392" t="inlineStr"/>
     </row>
     <row r="393">
       <c r="A393" t="inlineStr">
@@ -54275,6 +54669,7 @@
         <v>77789.78</v>
       </c>
       <c r="AQ393" t="inlineStr"/>
+      <c r="AR393" t="inlineStr"/>
     </row>
     <row r="394">
       <c r="A394" t="inlineStr">
@@ -54412,6 +54807,7 @@
         <v>117652.69</v>
       </c>
       <c r="AQ394" t="inlineStr"/>
+      <c r="AR394" t="inlineStr"/>
     </row>
     <row r="395">
       <c r="A395" t="inlineStr">
@@ -54549,6 +54945,7 @@
         <v>99126.60000000001</v>
       </c>
       <c r="AQ395" t="inlineStr"/>
+      <c r="AR395" t="inlineStr"/>
     </row>
     <row r="396">
       <c r="A396" t="inlineStr">
@@ -54686,6 +55083,7 @@
         <v>19331.08</v>
       </c>
       <c r="AQ396" t="inlineStr"/>
+      <c r="AR396" t="inlineStr"/>
     </row>
     <row r="397">
       <c r="A397" t="inlineStr">
@@ -54820,9 +55218,10 @@
         <v>13425363.81</v>
       </c>
       <c r="AP397" t="n">
-        <v>13438783</v>
+        <v>13326793.14</v>
       </c>
       <c r="AQ397" t="inlineStr"/>
+      <c r="AR397" t="inlineStr"/>
     </row>
     <row r="398">
       <c r="A398" t="inlineStr">
@@ -54957,9 +55356,10 @@
         <v>93198.98</v>
       </c>
       <c r="AP398" t="n">
-        <v>78939.5</v>
+        <v>93292.14</v>
       </c>
       <c r="AQ398" t="inlineStr"/>
+      <c r="AR398" t="inlineStr"/>
     </row>
     <row r="399">
       <c r="A399" t="inlineStr">
@@ -55097,6 +55497,7 @@
         <v>114326.63</v>
       </c>
       <c r="AQ399" t="inlineStr"/>
+      <c r="AR399" t="inlineStr"/>
     </row>
     <row r="400">
       <c r="A400" t="inlineStr">
@@ -55234,6 +55635,7 @@
         <v>105953.87</v>
       </c>
       <c r="AQ400" t="inlineStr"/>
+      <c r="AR400" t="inlineStr"/>
     </row>
     <row r="401">
       <c r="A401" t="inlineStr">
@@ -55368,9 +55770,10 @@
         <v>293799.09</v>
       </c>
       <c r="AP401" t="n">
-        <v>294092.75</v>
+        <v>265632.16</v>
       </c>
       <c r="AQ401" t="inlineStr"/>
+      <c r="AR401" t="inlineStr"/>
     </row>
     <row r="402">
       <c r="A402" t="inlineStr">
@@ -55508,6 +55911,7 @@
         <v>767846.64</v>
       </c>
       <c r="AQ402" t="inlineStr"/>
+      <c r="AR402" t="inlineStr"/>
     </row>
     <row r="403">
       <c r="A403" t="inlineStr">
@@ -55645,6 +56049,7 @@
         <v>383530.22</v>
       </c>
       <c r="AQ403" t="inlineStr"/>
+      <c r="AR403" t="inlineStr"/>
     </row>
     <row r="404">
       <c r="A404" t="inlineStr">
@@ -55779,9 +56184,10 @@
         <v>494464.91</v>
       </c>
       <c r="AP404" t="n">
-        <v>494959.15</v>
+        <v>478460.51</v>
       </c>
       <c r="AQ404" t="inlineStr"/>
+      <c r="AR404" t="inlineStr"/>
     </row>
     <row r="405">
       <c r="A405" t="inlineStr">
@@ -55919,6 +56325,7 @@
         <v>2814767.33</v>
       </c>
       <c r="AQ405" t="inlineStr"/>
+      <c r="AR405" t="inlineStr"/>
     </row>
     <row r="406">
       <c r="A406" t="inlineStr">
@@ -56053,9 +56460,10 @@
         <v>-6739.01</v>
       </c>
       <c r="AP406" t="n">
-        <v>-16864.37</v>
+        <v>-10118.62</v>
       </c>
       <c r="AQ406" t="inlineStr"/>
+      <c r="AR406" t="inlineStr"/>
     </row>
     <row r="407">
       <c r="A407" t="inlineStr">
@@ -56190,9 +56598,10 @@
         <v>0</v>
       </c>
       <c r="AP407" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AQ407" t="inlineStr"/>
+      <c r="AR407" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>